<commit_message>
changed report creation a bit
</commit_message>
<xml_diff>
--- a/Report.xlsx
+++ b/Report.xlsx
@@ -14,15 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>ce6881-48s6cq</t>
   </si>
   <si>
-    <t>EK008104 ekt-4</t>
-  </si>
-  <si>
-    <t>потом тут обязательно будут спецификации</t>
+    <t>EK008104</t>
+  </si>
+  <si>
+    <t>0%</t>
+  </si>
+  <si>
+    <t>specs</t>
   </si>
   <si>
     <t>r740xd</t>
@@ -31,13 +34,13 @@
     <t>os5300_v5</t>
   </si>
   <si>
-    <t>EK008105 ekt-5</t>
+    <t>EK008105</t>
   </si>
   <si>
     <t>dpd100-2-20</t>
   </si>
   <si>
-    <t>MS008101 msk-1</t>
+    <t>MS008101</t>
   </si>
 </sst>
 </file>
@@ -361,18 +364,18 @@
         <v>3</v>
       </c>
       <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -383,16 +386,16 @@
       <c r="D2">
         <v>0</v>
       </c>
-      <c r="E2">
-        <v>0</v>
+      <c r="E2" t="s">
+        <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -403,11 +406,11 @@
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3">
-        <v>0</v>
+      <c r="E3" t="s">
+        <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4">
@@ -415,27 +418,27 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C4">
         <v>6</v>
       </c>
       <c r="D4">
-        <v>6</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -443,19 +446,19 @@
       <c r="D5">
         <v>0</v>
       </c>
-      <c r="E5">
-        <v>0</v>
+      <c r="E5" t="s">
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C6">
         <v>17</v>
@@ -463,19 +466,19 @@
       <c r="D6">
         <v>0</v>
       </c>
-      <c r="E6">
-        <v>0</v>
+      <c r="E6" t="s">
+        <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -483,11 +486,11 @@
       <c r="D7">
         <v>0</v>
       </c>
-      <c r="E7">
-        <v>0</v>
+      <c r="E7" t="s">
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8">
@@ -495,27 +498,27 @@
         <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8">
-        <v>6</v>
-      </c>
-      <c r="E8">
-        <v>1.5</v>
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C9">
         <v>4</v>
@@ -523,11 +526,11 @@
       <c r="D9">
         <v>0</v>
       </c>
-      <c r="E9">
-        <v>0</v>
+      <c r="E9" t="s">
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>